<commit_message>
Web 121 / Quiz 01
</commit_message>
<xml_diff>
--- a/121/121.xlsx
+++ b/121/121.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MFT\004-scores\121\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33C48137-1B12-42A9-9028-46EE1277C4EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D93DBEA4-AB00-4358-8615-BD997AE7E57F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,6 +17,13 @@
   </sheets>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -25,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>No.</t>
   </si>
@@ -46,6 +53,9 @@
   </si>
   <si>
     <t>MFT</t>
+  </si>
+  <si>
+    <t>Q01</t>
   </si>
 </sst>
 </file>
@@ -124,7 +134,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -164,6 +174,10 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -549,7 +563,7 @@
   <dimension ref="A1:Z37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,7 +586,9 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -593,7 +609,9 @@
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="4"/>
+      <c r="B2" s="4">
+        <v>0</v>
+      </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -623,7 +641,9 @@
       <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="4"/>
+      <c r="B3" s="4">
+        <v>0</v>
+      </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
@@ -653,7 +673,10 @@
       <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B4" s="4">
+        <f>(6/10)*10</f>
+        <v>6</v>
+      </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -683,7 +706,10 @@
       <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" s="4"/>
+      <c r="B5" s="4">
+        <f>(7/10)*10</f>
+        <v>7</v>
+      </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
@@ -713,7 +739,10 @@
       <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="4"/>
+      <c r="B6" s="4">
+        <f>(6/10)*10</f>
+        <v>6</v>
+      </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -743,7 +772,10 @@
       <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7" s="6"/>
+      <c r="B7" s="6">
+        <f>(5/10)*10</f>
+        <v>5</v>
+      </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
@@ -773,7 +805,9 @@
       <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8" s="6"/>
+      <c r="B8" s="6">
+        <v>0</v>
+      </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
@@ -803,7 +837,9 @@
       <c r="A9" s="3">
         <v>8</v>
       </c>
-      <c r="B9" s="6"/>
+      <c r="B9" s="6">
+        <v>0</v>
+      </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
@@ -833,7 +869,10 @@
       <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="B10" s="6"/>
+      <c r="B10" s="6">
+        <f>(7/10)*10</f>
+        <v>7</v>
+      </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
@@ -863,7 +902,10 @@
       <c r="A11" s="3">
         <v>10</v>
       </c>
-      <c r="B11" s="6"/>
+      <c r="B11" s="6">
+        <f>(7/10)*10</f>
+        <v>7</v>
+      </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
@@ -893,7 +935,10 @@
       <c r="A12" s="3">
         <v>11</v>
       </c>
-      <c r="B12" s="6"/>
+      <c r="B12" s="6">
+        <f>(2/10)*10</f>
+        <v>2</v>
+      </c>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
@@ -923,7 +968,10 @@
       <c r="A13" s="3">
         <v>12</v>
       </c>
-      <c r="B13" s="6"/>
+      <c r="B13" s="6">
+        <f>(6/10)*10</f>
+        <v>6</v>
+      </c>
       <c r="C13" s="6"/>
       <c r="D13" s="4"/>
       <c r="E13" s="6"/>
@@ -953,7 +1001,10 @@
       <c r="A14" s="3">
         <v>13</v>
       </c>
-      <c r="B14" s="6"/>
+      <c r="B14" s="6">
+        <f>(4/10)*10</f>
+        <v>4</v>
+      </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
@@ -983,7 +1034,9 @@
       <c r="A15" s="3">
         <v>14</v>
       </c>
-      <c r="B15" s="6"/>
+      <c r="B15" s="6">
+        <v>0</v>
+      </c>
       <c r="C15" s="6"/>
       <c r="D15" s="18"/>
       <c r="E15" s="6"/>
@@ -1043,7 +1096,7 @@
       </c>
       <c r="B17" s="8">
         <f>COUNTA(B1:Q1) * 10</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -1099,9 +1152,9 @@
       <c r="A22" s="10">
         <v>1</v>
       </c>
-      <c r="B22" s="13" t="e">
+      <c r="B22" s="13">
         <f>(SUM(B2:R2)/B17) * 40</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="C22" s="14">
         <v>0</v>
@@ -1109,22 +1162,22 @@
       <c r="D22" s="14">
         <v>0</v>
       </c>
-      <c r="E22" s="15" t="e">
+      <c r="E22" s="15">
         <f>B22+C22+D22</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F22" s="16" t="e">
+        <v>0</v>
+      </c>
+      <c r="F22" s="16">
         <f t="shared" ref="F22:F36" si="0">E22</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" s="10">
         <v>2</v>
       </c>
-      <c r="B23" s="13" t="e">
+      <c r="B23" s="13">
         <f>(SUM(B3:R3)/B17) * 40</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="C23" s="14">
         <v>0</v>
@@ -1132,22 +1185,22 @@
       <c r="D23" s="14">
         <v>0</v>
       </c>
-      <c r="E23" s="15" t="e">
+      <c r="E23" s="15">
         <f t="shared" ref="E23:E36" si="1">B23+C23+D23</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F23" s="16" t="e">
+        <v>0</v>
+      </c>
+      <c r="F23" s="16">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
         <v>3</v>
       </c>
-      <c r="B24" s="13" t="e">
+      <c r="B24" s="13">
         <f>(SUM(B4:R4)/B17) * 40</f>
-        <v>#DIV/0!</v>
+        <v>24</v>
       </c>
       <c r="C24" s="14">
         <v>0</v>
@@ -1155,22 +1208,22 @@
       <c r="D24" s="14">
         <v>0</v>
       </c>
-      <c r="E24" s="15" t="e">
+      <c r="E24" s="15">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F24" s="16" t="e">
+        <v>24</v>
+      </c>
+      <c r="F24" s="16">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
         <v>4</v>
       </c>
-      <c r="B25" s="13" t="e">
+      <c r="B25" s="13">
         <f>(SUM(B5:R5)/B17) * 40</f>
-        <v>#DIV/0!</v>
+        <v>28</v>
       </c>
       <c r="C25" s="14">
         <v>0</v>
@@ -1178,22 +1231,22 @@
       <c r="D25" s="14">
         <v>0</v>
       </c>
-      <c r="E25" s="15" t="e">
+      <c r="E25" s="15">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F25" s="16" t="e">
+        <v>28</v>
+      </c>
+      <c r="F25" s="16">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" s="10">
         <v>5</v>
       </c>
-      <c r="B26" s="13" t="e">
+      <c r="B26" s="13">
         <f>(SUM(B6:R6)/B17) * 40</f>
-        <v>#DIV/0!</v>
+        <v>24</v>
       </c>
       <c r="C26" s="14">
         <v>0</v>
@@ -1201,22 +1254,22 @@
       <c r="D26" s="14">
         <v>0</v>
       </c>
-      <c r="E26" s="15" t="e">
+      <c r="E26" s="15">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F26" s="16" t="e">
+        <v>24</v>
+      </c>
+      <c r="F26" s="16">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
         <v>6</v>
       </c>
-      <c r="B27" s="13" t="e">
+      <c r="B27" s="13">
         <f>(SUM(B7:R7)/B17) * 40</f>
-        <v>#DIV/0!</v>
+        <v>20</v>
       </c>
       <c r="C27" s="14">
         <v>0</v>
@@ -1224,22 +1277,22 @@
       <c r="D27" s="14">
         <v>0</v>
       </c>
-      <c r="E27" s="15" t="e">
+      <c r="E27" s="15">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F27" s="16" t="e">
+        <v>20</v>
+      </c>
+      <c r="F27" s="16">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A28" s="10">
         <v>7</v>
       </c>
-      <c r="B28" s="13" t="e">
+      <c r="B28" s="13">
         <f>(SUM(B8:R8)/B17) * 40</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="C28" s="14">
         <v>0</v>
@@ -1247,22 +1300,22 @@
       <c r="D28" s="14">
         <v>0</v>
       </c>
-      <c r="E28" s="15" t="e">
+      <c r="E28" s="15">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F28" s="16" t="e">
+        <v>0</v>
+      </c>
+      <c r="F28" s="16">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A29" s="10">
         <v>8</v>
       </c>
-      <c r="B29" s="13" t="e">
+      <c r="B29" s="13">
         <f>(SUM(B9:R9)/B17) * 40</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="C29" s="14">
         <v>0</v>
@@ -1270,22 +1323,22 @@
       <c r="D29" s="14">
         <v>0</v>
       </c>
-      <c r="E29" s="15" t="e">
+      <c r="E29" s="15">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F29" s="16" t="e">
+        <v>0</v>
+      </c>
+      <c r="F29" s="16">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
         <v>9</v>
       </c>
-      <c r="B30" s="13" t="e">
+      <c r="B30" s="13">
         <f>(SUM(B10:R10)/B17) * 40</f>
-        <v>#DIV/0!</v>
+        <v>28</v>
       </c>
       <c r="C30" s="14">
         <v>0</v>
@@ -1293,22 +1346,22 @@
       <c r="D30" s="14">
         <v>0</v>
       </c>
-      <c r="E30" s="15" t="e">
+      <c r="E30" s="15">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F30" s="16" t="e">
+        <v>28</v>
+      </c>
+      <c r="F30" s="16">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A31" s="10">
         <v>10</v>
       </c>
-      <c r="B31" s="13" t="e">
+      <c r="B31" s="13">
         <f>(SUM(B11:R11)/B17) * 40</f>
-        <v>#DIV/0!</v>
+        <v>28</v>
       </c>
       <c r="C31" s="14">
         <v>0</v>
@@ -1316,22 +1369,22 @@
       <c r="D31" s="14">
         <v>0</v>
       </c>
-      <c r="E31" s="15" t="e">
+      <c r="E31" s="15">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F31" s="16" t="e">
+        <v>28</v>
+      </c>
+      <c r="F31" s="16">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A32" s="10">
         <v>11</v>
       </c>
-      <c r="B32" s="13" t="e">
+      <c r="B32" s="13">
         <f>(SUM(B12:R12)/B17) * 40</f>
-        <v>#DIV/0!</v>
+        <v>8</v>
       </c>
       <c r="C32" s="14">
         <v>0</v>
@@ -1339,22 +1392,22 @@
       <c r="D32" s="14">
         <v>0</v>
       </c>
-      <c r="E32" s="15" t="e">
+      <c r="E32" s="15">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F32" s="16" t="e">
+        <v>8</v>
+      </c>
+      <c r="F32" s="16">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="10">
         <v>12</v>
       </c>
-      <c r="B33" s="13" t="e">
+      <c r="B33" s="13">
         <f>(SUM(B13:R13)/B17) * 40</f>
-        <v>#DIV/0!</v>
+        <v>24</v>
       </c>
       <c r="C33" s="14">
         <v>0</v>
@@ -1362,22 +1415,22 @@
       <c r="D33" s="14">
         <v>0</v>
       </c>
-      <c r="E33" s="15" t="e">
+      <c r="E33" s="15">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F33" s="16" t="e">
+        <v>24</v>
+      </c>
+      <c r="F33" s="16">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>24</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="10">
         <v>13</v>
       </c>
-      <c r="B34" s="13" t="e">
+      <c r="B34" s="13">
         <f>(SUM(B14:R14)/B17) * 40</f>
-        <v>#DIV/0!</v>
+        <v>16</v>
       </c>
       <c r="C34" s="14">
         <v>0</v>
@@ -1385,22 +1438,22 @@
       <c r="D34" s="14">
         <v>0</v>
       </c>
-      <c r="E34" s="15" t="e">
+      <c r="E34" s="15">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F34" s="16" t="e">
+        <v>16</v>
+      </c>
+      <c r="F34" s="16">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>16</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="10">
         <v>14</v>
       </c>
-      <c r="B35" s="13" t="e">
+      <c r="B35" s="13">
         <f>(SUM(B15:R15)/B17) * 40</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="C35" s="14">
         <v>0</v>
@@ -1408,37 +1461,22 @@
       <c r="D35" s="14">
         <v>0</v>
       </c>
-      <c r="E35" s="15" t="e">
+      <c r="E35" s="15">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F35" s="16" t="e">
+        <v>0</v>
+      </c>
+      <c r="F35" s="16">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="10">
-        <v>15</v>
-      </c>
-      <c r="B36" s="13" t="e">
-        <f>(SUM(B16:R16)/B17) * 40</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C36" s="14">
-        <v>0</v>
-      </c>
-      <c r="D36" s="14">
-        <v>0</v>
-      </c>
-      <c r="E36" s="15" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F36" s="16" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="A36" s="19"/>
+      <c r="B36" s="20"/>
+      <c r="C36" s="20"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="22"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="17"/>

</xml_diff>

<commit_message>
web 121 / quiz 02
</commit_message>
<xml_diff>
--- a/121/121.xlsx
+++ b/121/121.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MFT\004-scores\121\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D93DBEA4-AB00-4358-8615-BD997AE7E57F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69078C52-0A38-4F37-92DC-9F825AD6590B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3135" yWindow="2640" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="web 121" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>No.</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t>Q01</t>
+  </si>
+  <si>
+    <t>Q02</t>
   </si>
 </sst>
 </file>
@@ -563,7 +566,7 @@
   <dimension ref="A1:Z37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -589,7 +592,9 @@
       <c r="B1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="2"/>
+      <c r="C1" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -612,7 +617,10 @@
       <c r="B2" s="4">
         <v>0</v>
       </c>
-      <c r="C2" s="4"/>
+      <c r="C2" s="4">
+        <f>(6/12)*10</f>
+        <v>5</v>
+      </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
@@ -644,7 +652,9 @@
       <c r="B3" s="4">
         <v>0</v>
       </c>
-      <c r="C3" s="4"/>
+      <c r="C3" s="4">
+        <v>0</v>
+      </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
@@ -677,7 +687,10 @@
         <f>(6/10)*10</f>
         <v>6</v>
       </c>
-      <c r="C4" s="4"/>
+      <c r="C4" s="4">
+        <f>(7/12)*10</f>
+        <v>5.8333333333333339</v>
+      </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
@@ -710,7 +723,10 @@
         <f>(7/10)*10</f>
         <v>7</v>
       </c>
-      <c r="C5" s="4"/>
+      <c r="C5" s="4">
+        <f>(8/12)*10</f>
+        <v>6.6666666666666661</v>
+      </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
@@ -743,7 +759,10 @@
         <f>(6/10)*10</f>
         <v>6</v>
       </c>
-      <c r="C6" s="4"/>
+      <c r="C6" s="4">
+        <f>(8/12)*10</f>
+        <v>6.6666666666666661</v>
+      </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
@@ -776,7 +795,10 @@
         <f>(5/10)*10</f>
         <v>5</v>
       </c>
-      <c r="C7" s="6"/>
+      <c r="C7" s="6">
+        <f>(10/12)*10</f>
+        <v>8.3333333333333339</v>
+      </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
@@ -808,7 +830,9 @@
       <c r="B8" s="6">
         <v>0</v>
       </c>
-      <c r="C8" s="6"/>
+      <c r="C8" s="6">
+        <v>0</v>
+      </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
@@ -840,7 +864,10 @@
       <c r="B9" s="6">
         <v>0</v>
       </c>
-      <c r="C9" s="6"/>
+      <c r="C9" s="6">
+        <f>(6/12)*10</f>
+        <v>5</v>
+      </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -873,7 +900,10 @@
         <f>(7/10)*10</f>
         <v>7</v>
       </c>
-      <c r="C10" s="6"/>
+      <c r="C10" s="6">
+        <f>(7/12)*10</f>
+        <v>5.8333333333333339</v>
+      </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
@@ -906,7 +936,10 @@
         <f>(7/10)*10</f>
         <v>7</v>
       </c>
-      <c r="C11" s="6"/>
+      <c r="C11" s="6">
+        <f>(7/12)*10</f>
+        <v>5.8333333333333339</v>
+      </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
@@ -939,7 +972,10 @@
         <f>(2/10)*10</f>
         <v>2</v>
       </c>
-      <c r="C12" s="6"/>
+      <c r="C12" s="6">
+        <f>(5/12)*10</f>
+        <v>4.166666666666667</v>
+      </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
@@ -972,7 +1008,10 @@
         <f>(6/10)*10</f>
         <v>6</v>
       </c>
-      <c r="C13" s="6"/>
+      <c r="C13" s="6">
+        <f>(5/12)*10</f>
+        <v>4.166666666666667</v>
+      </c>
       <c r="D13" s="4"/>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
@@ -1005,7 +1044,10 @@
         <f>(4/10)*10</f>
         <v>4</v>
       </c>
-      <c r="C14" s="6"/>
+      <c r="C14" s="6">
+        <f>(5/12)*10</f>
+        <v>4.166666666666667</v>
+      </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
@@ -1037,7 +1079,10 @@
       <c r="B15" s="6">
         <v>0</v>
       </c>
-      <c r="C15" s="6"/>
+      <c r="C15" s="6">
+        <f>(9/12)*10</f>
+        <v>7.5</v>
+      </c>
       <c r="D15" s="18"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
@@ -1096,7 +1141,7 @@
       </c>
       <c r="B17" s="8">
         <f>COUNTA(B1:Q1) * 10</f>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -1154,7 +1199,7 @@
       </c>
       <c r="B22" s="13">
         <f>(SUM(B2:R2)/B17) * 40</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C22" s="14">
         <v>0</v>
@@ -1164,11 +1209,11 @@
       </c>
       <c r="E22" s="15">
         <f>B22+C22+D22</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F22" s="16">
-        <f t="shared" ref="F22:F36" si="0">E22</f>
-        <v>0</v>
+        <f t="shared" ref="F22:F35" si="0">E22</f>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
@@ -1186,7 +1231,7 @@
         <v>0</v>
       </c>
       <c r="E23" s="15">
-        <f t="shared" ref="E23:E36" si="1">B23+C23+D23</f>
+        <f t="shared" ref="E23:E35" si="1">B23+C23+D23</f>
         <v>0</v>
       </c>
       <c r="F23" s="16">
@@ -1200,7 +1245,7 @@
       </c>
       <c r="B24" s="13">
         <f>(SUM(B4:R4)/B17) * 40</f>
-        <v>24</v>
+        <v>23.666666666666668</v>
       </c>
       <c r="C24" s="14">
         <v>0</v>
@@ -1210,11 +1255,11 @@
       </c>
       <c r="E24" s="15">
         <f t="shared" si="1"/>
-        <v>24</v>
+        <v>23.666666666666668</v>
       </c>
       <c r="F24" s="16">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>23.666666666666668</v>
       </c>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.25">
@@ -1223,7 +1268,7 @@
       </c>
       <c r="B25" s="13">
         <f>(SUM(B5:R5)/B17) * 40</f>
-        <v>28</v>
+        <v>27.333333333333336</v>
       </c>
       <c r="C25" s="14">
         <v>0</v>
@@ -1233,11 +1278,11 @@
       </c>
       <c r="E25" s="15">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>27.333333333333336</v>
       </c>
       <c r="F25" s="16">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>27.333333333333336</v>
       </c>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
@@ -1246,7 +1291,7 @@
       </c>
       <c r="B26" s="13">
         <f>(SUM(B6:R6)/B17) * 40</f>
-        <v>24</v>
+        <v>25.333333333333332</v>
       </c>
       <c r="C26" s="14">
         <v>0</v>
@@ -1256,11 +1301,11 @@
       </c>
       <c r="E26" s="15">
         <f t="shared" si="1"/>
-        <v>24</v>
+        <v>25.333333333333332</v>
       </c>
       <c r="F26" s="16">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>25.333333333333332</v>
       </c>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.25">
@@ -1269,7 +1314,7 @@
       </c>
       <c r="B27" s="13">
         <f>(SUM(B7:R7)/B17) * 40</f>
-        <v>20</v>
+        <v>26.666666666666671</v>
       </c>
       <c r="C27" s="14">
         <v>0</v>
@@ -1279,11 +1324,11 @@
       </c>
       <c r="E27" s="15">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>26.666666666666671</v>
       </c>
       <c r="F27" s="16">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>26.666666666666671</v>
       </c>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.25">
@@ -1315,7 +1360,7 @@
       </c>
       <c r="B29" s="13">
         <f>(SUM(B9:R9)/B17) * 40</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C29" s="14">
         <v>0</v>
@@ -1325,11 +1370,11 @@
       </c>
       <c r="E29" s="15">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F29" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.25">
@@ -1338,7 +1383,7 @@
       </c>
       <c r="B30" s="13">
         <f>(SUM(B10:R10)/B17) * 40</f>
-        <v>28</v>
+        <v>25.666666666666668</v>
       </c>
       <c r="C30" s="14">
         <v>0</v>
@@ -1348,11 +1393,11 @@
       </c>
       <c r="E30" s="15">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>25.666666666666668</v>
       </c>
       <c r="F30" s="16">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>25.666666666666668</v>
       </c>
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.25">
@@ -1361,7 +1406,7 @@
       </c>
       <c r="B31" s="13">
         <f>(SUM(B11:R11)/B17) * 40</f>
-        <v>28</v>
+        <v>25.666666666666668</v>
       </c>
       <c r="C31" s="14">
         <v>0</v>
@@ -1371,11 +1416,11 @@
       </c>
       <c r="E31" s="15">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>25.666666666666668</v>
       </c>
       <c r="F31" s="16">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>25.666666666666668</v>
       </c>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.25">
@@ -1384,7 +1429,7 @@
       </c>
       <c r="B32" s="13">
         <f>(SUM(B12:R12)/B17) * 40</f>
-        <v>8</v>
+        <v>12.333333333333334</v>
       </c>
       <c r="C32" s="14">
         <v>0</v>
@@ -1394,11 +1439,11 @@
       </c>
       <c r="E32" s="15">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>12.333333333333334</v>
       </c>
       <c r="F32" s="16">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>12.333333333333334</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1407,7 +1452,7 @@
       </c>
       <c r="B33" s="13">
         <f>(SUM(B13:R13)/B17) * 40</f>
-        <v>24</v>
+        <v>20.333333333333336</v>
       </c>
       <c r="C33" s="14">
         <v>0</v>
@@ -1417,11 +1462,11 @@
       </c>
       <c r="E33" s="15">
         <f t="shared" si="1"/>
-        <v>24</v>
+        <v>20.333333333333336</v>
       </c>
       <c r="F33" s="16">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>20.333333333333336</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1430,7 +1475,7 @@
       </c>
       <c r="B34" s="13">
         <f>(SUM(B14:R14)/B17) * 40</f>
-        <v>16</v>
+        <v>16.333333333333336</v>
       </c>
       <c r="C34" s="14">
         <v>0</v>
@@ -1440,11 +1485,11 @@
       </c>
       <c r="E34" s="15">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>16.333333333333336</v>
       </c>
       <c r="F34" s="16">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>16.333333333333336</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1453,7 +1498,7 @@
       </c>
       <c r="B35" s="13">
         <f>(SUM(B15:R15)/B17) * 40</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C35" s="14">
         <v>0</v>
@@ -1463,11 +1508,11 @@
       </c>
       <c r="E35" s="15">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="F35" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
web 121 / quiz 03
</commit_message>
<xml_diff>
--- a/121/121.xlsx
+++ b/121/121.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MFT\004-scores\121\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69078C52-0A38-4F37-92DC-9F825AD6590B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF9A9C7-6BA6-45A0-AD14-24F4CBBF9FAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3135" yWindow="2640" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="web 121" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>No.</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t>Q02</t>
+  </si>
+  <si>
+    <t>Q03</t>
   </si>
 </sst>
 </file>
@@ -566,7 +569,7 @@
   <dimension ref="A1:Z37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,7 +598,9 @@
       <c r="C1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="2"/>
+      <c r="D1" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -621,7 +626,10 @@
         <f>(6/12)*10</f>
         <v>5</v>
       </c>
-      <c r="D2" s="4"/>
+      <c r="D2" s="4">
+        <f>(12/20)*10</f>
+        <v>6</v>
+      </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
@@ -655,7 +663,10 @@
       <c r="C3" s="4">
         <v>0</v>
       </c>
-      <c r="D3" s="4"/>
+      <c r="D3" s="4">
+        <f>(7/20)*10</f>
+        <v>3.5</v>
+      </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
@@ -691,7 +702,10 @@
         <f>(7/12)*10</f>
         <v>5.8333333333333339</v>
       </c>
-      <c r="D4" s="4"/>
+      <c r="D4" s="4">
+        <f>(12/20)*10</f>
+        <v>6</v>
+      </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
@@ -727,7 +741,10 @@
         <f>(8/12)*10</f>
         <v>6.6666666666666661</v>
       </c>
-      <c r="D5" s="4"/>
+      <c r="D5" s="4">
+        <f>(10/20)*10</f>
+        <v>5</v>
+      </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
@@ -763,7 +780,10 @@
         <f>(8/12)*10</f>
         <v>6.6666666666666661</v>
       </c>
-      <c r="D6" s="4"/>
+      <c r="D6" s="4">
+        <f>(11/20)*10</f>
+        <v>5.5</v>
+      </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
@@ -799,7 +819,10 @@
         <f>(10/12)*10</f>
         <v>8.3333333333333339</v>
       </c>
-      <c r="D7" s="6"/>
+      <c r="D7" s="6">
+        <f>(16/20)*10</f>
+        <v>8</v>
+      </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
@@ -833,7 +856,9 @@
       <c r="C8" s="6">
         <v>0</v>
       </c>
-      <c r="D8" s="6"/>
+      <c r="D8" s="6">
+        <v>0</v>
+      </c>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
@@ -868,7 +893,9 @@
         <f>(6/12)*10</f>
         <v>5</v>
       </c>
-      <c r="D9" s="6"/>
+      <c r="D9" s="6">
+        <v>0</v>
+      </c>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
@@ -904,7 +931,9 @@
         <f>(7/12)*10</f>
         <v>5.8333333333333339</v>
       </c>
-      <c r="D10" s="6"/>
+      <c r="D10" s="6">
+        <v>0</v>
+      </c>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
@@ -940,7 +969,10 @@
         <f>(7/12)*10</f>
         <v>5.8333333333333339</v>
       </c>
-      <c r="D11" s="6"/>
+      <c r="D11" s="6">
+        <f>(13/20)*10</f>
+        <v>6.5</v>
+      </c>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
@@ -976,7 +1008,10 @@
         <f>(5/12)*10</f>
         <v>4.166666666666667</v>
       </c>
-      <c r="D12" s="6"/>
+      <c r="D12" s="6">
+        <f>(6/20)*10</f>
+        <v>3</v>
+      </c>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
@@ -1012,7 +1047,10 @@
         <f>(5/12)*10</f>
         <v>4.166666666666667</v>
       </c>
-      <c r="D13" s="4"/>
+      <c r="D13" s="4">
+        <f>(13/20)*10</f>
+        <v>6.5</v>
+      </c>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
@@ -1048,7 +1086,9 @@
         <f>(5/12)*10</f>
         <v>4.166666666666667</v>
       </c>
-      <c r="D14" s="6"/>
+      <c r="D14" s="6">
+        <v>0</v>
+      </c>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
@@ -1083,7 +1123,9 @@
         <f>(9/12)*10</f>
         <v>7.5</v>
       </c>
-      <c r="D15" s="18"/>
+      <c r="D15" s="18">
+        <v>0</v>
+      </c>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
@@ -1141,7 +1183,7 @@
       </c>
       <c r="B17" s="8">
         <f>COUNTA(B1:Q1) * 10</f>
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -1199,7 +1241,7 @@
       </c>
       <c r="B22" s="13">
         <f>(SUM(B2:R2)/B17) * 40</f>
-        <v>10</v>
+        <v>14.666666666666666</v>
       </c>
       <c r="C22" s="14">
         <v>0</v>
@@ -1209,11 +1251,11 @@
       </c>
       <c r="E22" s="15">
         <f>B22+C22+D22</f>
-        <v>10</v>
+        <v>14.666666666666666</v>
       </c>
       <c r="F22" s="16">
         <f t="shared" ref="F22:F35" si="0">E22</f>
-        <v>10</v>
+        <v>14.666666666666666</v>
       </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
@@ -1222,7 +1264,7 @@
       </c>
       <c r="B23" s="13">
         <f>(SUM(B3:R3)/B17) * 40</f>
-        <v>0</v>
+        <v>4.666666666666667</v>
       </c>
       <c r="C23" s="14">
         <v>0</v>
@@ -1232,11 +1274,11 @@
       </c>
       <c r="E23" s="15">
         <f t="shared" ref="E23:E35" si="1">B23+C23+D23</f>
-        <v>0</v>
+        <v>4.666666666666667</v>
       </c>
       <c r="F23" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.666666666666667</v>
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
@@ -1245,7 +1287,7 @@
       </c>
       <c r="B24" s="13">
         <f>(SUM(B4:R4)/B17) * 40</f>
-        <v>23.666666666666668</v>
+        <v>23.777777777777782</v>
       </c>
       <c r="C24" s="14">
         <v>0</v>
@@ -1255,11 +1297,11 @@
       </c>
       <c r="E24" s="15">
         <f t="shared" si="1"/>
-        <v>23.666666666666668</v>
+        <v>23.777777777777782</v>
       </c>
       <c r="F24" s="16">
         <f t="shared" si="0"/>
-        <v>23.666666666666668</v>
+        <v>23.777777777777782</v>
       </c>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.25">
@@ -1268,7 +1310,7 @@
       </c>
       <c r="B25" s="13">
         <f>(SUM(B5:R5)/B17) * 40</f>
-        <v>27.333333333333336</v>
+        <v>24.888888888888886</v>
       </c>
       <c r="C25" s="14">
         <v>0</v>
@@ -1278,11 +1320,11 @@
       </c>
       <c r="E25" s="15">
         <f t="shared" si="1"/>
-        <v>27.333333333333336</v>
+        <v>24.888888888888886</v>
       </c>
       <c r="F25" s="16">
         <f t="shared" si="0"/>
-        <v>27.333333333333336</v>
+        <v>24.888888888888886</v>
       </c>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
@@ -1291,7 +1333,7 @@
       </c>
       <c r="B26" s="13">
         <f>(SUM(B6:R6)/B17) * 40</f>
-        <v>25.333333333333332</v>
+        <v>24.222222222222221</v>
       </c>
       <c r="C26" s="14">
         <v>0</v>
@@ -1301,11 +1343,11 @@
       </c>
       <c r="E26" s="15">
         <f t="shared" si="1"/>
-        <v>25.333333333333332</v>
+        <v>24.222222222222221</v>
       </c>
       <c r="F26" s="16">
         <f t="shared" si="0"/>
-        <v>25.333333333333332</v>
+        <v>24.222222222222221</v>
       </c>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.25">
@@ -1314,7 +1356,7 @@
       </c>
       <c r="B27" s="13">
         <f>(SUM(B7:R7)/B17) * 40</f>
-        <v>26.666666666666671</v>
+        <v>28.444444444444446</v>
       </c>
       <c r="C27" s="14">
         <v>0</v>
@@ -1324,11 +1366,11 @@
       </c>
       <c r="E27" s="15">
         <f t="shared" si="1"/>
-        <v>26.666666666666671</v>
+        <v>28.444444444444446</v>
       </c>
       <c r="F27" s="16">
         <f t="shared" si="0"/>
-        <v>26.666666666666671</v>
+        <v>28.444444444444446</v>
       </c>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.25">
@@ -1360,7 +1402,7 @@
       </c>
       <c r="B29" s="13">
         <f>(SUM(B9:R9)/B17) * 40</f>
-        <v>10</v>
+        <v>6.6666666666666661</v>
       </c>
       <c r="C29" s="14">
         <v>0</v>
@@ -1370,11 +1412,11 @@
       </c>
       <c r="E29" s="15">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>6.6666666666666661</v>
       </c>
       <c r="F29" s="16">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>6.6666666666666661</v>
       </c>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.25">
@@ -1383,7 +1425,7 @@
       </c>
       <c r="B30" s="13">
         <f>(SUM(B10:R10)/B17) * 40</f>
-        <v>25.666666666666668</v>
+        <v>17.111111111111114</v>
       </c>
       <c r="C30" s="14">
         <v>0</v>
@@ -1393,11 +1435,11 @@
       </c>
       <c r="E30" s="15">
         <f t="shared" si="1"/>
-        <v>25.666666666666668</v>
+        <v>17.111111111111114</v>
       </c>
       <c r="F30" s="16">
         <f t="shared" si="0"/>
-        <v>25.666666666666668</v>
+        <v>17.111111111111114</v>
       </c>
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.25">
@@ -1406,7 +1448,7 @@
       </c>
       <c r="B31" s="13">
         <f>(SUM(B11:R11)/B17) * 40</f>
-        <v>25.666666666666668</v>
+        <v>25.777777777777779</v>
       </c>
       <c r="C31" s="14">
         <v>0</v>
@@ -1416,11 +1458,11 @@
       </c>
       <c r="E31" s="15">
         <f t="shared" si="1"/>
-        <v>25.666666666666668</v>
+        <v>25.777777777777779</v>
       </c>
       <c r="F31" s="16">
         <f t="shared" si="0"/>
-        <v>25.666666666666668</v>
+        <v>25.777777777777779</v>
       </c>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.25">
@@ -1429,7 +1471,7 @@
       </c>
       <c r="B32" s="13">
         <f>(SUM(B12:R12)/B17) * 40</f>
-        <v>12.333333333333334</v>
+        <v>12.222222222222223</v>
       </c>
       <c r="C32" s="14">
         <v>0</v>
@@ -1439,11 +1481,11 @@
       </c>
       <c r="E32" s="15">
         <f t="shared" si="1"/>
-        <v>12.333333333333334</v>
+        <v>12.222222222222223</v>
       </c>
       <c r="F32" s="16">
         <f t="shared" si="0"/>
-        <v>12.333333333333334</v>
+        <v>12.222222222222223</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1452,7 +1494,7 @@
       </c>
       <c r="B33" s="13">
         <f>(SUM(B13:R13)/B17) * 40</f>
-        <v>20.333333333333336</v>
+        <v>22.222222222222221</v>
       </c>
       <c r="C33" s="14">
         <v>0</v>
@@ -1462,11 +1504,11 @@
       </c>
       <c r="E33" s="15">
         <f t="shared" si="1"/>
-        <v>20.333333333333336</v>
+        <v>22.222222222222221</v>
       </c>
       <c r="F33" s="16">
         <f t="shared" si="0"/>
-        <v>20.333333333333336</v>
+        <v>22.222222222222221</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1475,7 +1517,7 @@
       </c>
       <c r="B34" s="13">
         <f>(SUM(B14:R14)/B17) * 40</f>
-        <v>16.333333333333336</v>
+        <v>10.888888888888889</v>
       </c>
       <c r="C34" s="14">
         <v>0</v>
@@ -1485,11 +1527,11 @@
       </c>
       <c r="E34" s="15">
         <f t="shared" si="1"/>
-        <v>16.333333333333336</v>
+        <v>10.888888888888889</v>
       </c>
       <c r="F34" s="16">
         <f t="shared" si="0"/>
-        <v>16.333333333333336</v>
+        <v>10.888888888888889</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1498,7 +1540,7 @@
       </c>
       <c r="B35" s="13">
         <f>(SUM(B15:R15)/B17) * 40</f>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C35" s="14">
         <v>0</v>
@@ -1508,11 +1550,11 @@
       </c>
       <c r="E35" s="15">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F35" s="16">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
web 121 / H04 - H05 - H06 - H09
</commit_message>
<xml_diff>
--- a/121/121.xlsx
+++ b/121/121.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MFT\004-scores\121\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF9A9C7-6BA6-45A0-AD14-24F4CBBF9FAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF97B7EC-7D3F-4985-9863-7C2A9F579783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>No.</t>
   </si>
@@ -62,6 +62,21 @@
   </si>
   <si>
     <t>Q03</t>
+  </si>
+  <si>
+    <t>H04</t>
+  </si>
+  <si>
+    <t>H05</t>
+  </si>
+  <si>
+    <t>H06</t>
+  </si>
+  <si>
+    <t>H09</t>
+  </si>
+  <si>
+    <t>H11</t>
   </si>
 </sst>
 </file>
@@ -569,7 +584,7 @@
   <dimension ref="A1:Z37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,11 +616,21 @@
       <c r="D1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
+      <c r="E1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
@@ -630,11 +655,21 @@
         <f>(12/20)*10</f>
         <v>6</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
+      <c r="E2" s="4">
+        <v>8.5</v>
+      </c>
+      <c r="F2" s="4">
+        <v>10</v>
+      </c>
+      <c r="G2" s="4">
+        <v>9</v>
+      </c>
+      <c r="H2" s="4">
+        <v>9.5</v>
+      </c>
+      <c r="I2" s="4">
+        <v>10</v>
+      </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
@@ -667,11 +702,21 @@
         <f>(7/20)*10</f>
         <v>3.5</v>
       </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
+      <c r="E3" s="4">
+        <v>8.5</v>
+      </c>
+      <c r="F3" s="4">
+        <v>9.5</v>
+      </c>
+      <c r="G3" s="4">
+        <v>0</v>
+      </c>
+      <c r="H3" s="4">
+        <v>0</v>
+      </c>
+      <c r="I3" s="4">
+        <v>0</v>
+      </c>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
@@ -706,11 +751,21 @@
         <f>(12/20)*10</f>
         <v>6</v>
       </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
+      <c r="E4" s="4">
+        <v>9.5</v>
+      </c>
+      <c r="F4" s="4">
+        <v>10</v>
+      </c>
+      <c r="G4" s="4">
+        <v>7</v>
+      </c>
+      <c r="H4" s="4">
+        <v>9.5</v>
+      </c>
+      <c r="I4" s="4">
+        <v>0</v>
+      </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
@@ -745,11 +800,21 @@
         <f>(10/20)*10</f>
         <v>5</v>
       </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
+      <c r="E5" s="4">
+        <v>10</v>
+      </c>
+      <c r="F5" s="4">
+        <v>11</v>
+      </c>
+      <c r="G5" s="4">
+        <v>10</v>
+      </c>
+      <c r="H5" s="4">
+        <v>0</v>
+      </c>
+      <c r="I5" s="4">
+        <v>0</v>
+      </c>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
@@ -784,11 +849,21 @@
         <f>(11/20)*10</f>
         <v>5.5</v>
       </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
+      <c r="E6" s="4">
+        <v>10</v>
+      </c>
+      <c r="F6" s="4">
+        <v>11</v>
+      </c>
+      <c r="G6" s="4">
+        <v>10</v>
+      </c>
+      <c r="H6" s="4">
+        <v>11</v>
+      </c>
+      <c r="I6" s="4">
+        <v>10</v>
+      </c>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
@@ -823,11 +898,21 @@
         <f>(16/20)*10</f>
         <v>8</v>
       </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
+      <c r="E7" s="6">
+        <v>10</v>
+      </c>
+      <c r="F7" s="6">
+        <v>11</v>
+      </c>
+      <c r="G7" s="6">
+        <v>10</v>
+      </c>
+      <c r="H7" s="6">
+        <v>10</v>
+      </c>
+      <c r="I7" s="6">
+        <v>10</v>
+      </c>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
@@ -859,11 +944,21 @@
       <c r="D8" s="6">
         <v>0</v>
       </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
+      <c r="E8" s="6">
+        <v>0</v>
+      </c>
+      <c r="F8" s="6">
+        <v>0</v>
+      </c>
+      <c r="G8" s="6">
+        <v>0</v>
+      </c>
+      <c r="H8" s="6">
+        <v>0</v>
+      </c>
+      <c r="I8" s="6">
+        <v>0</v>
+      </c>
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
@@ -896,11 +991,21 @@
       <c r="D9" s="6">
         <v>0</v>
       </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
+      <c r="E9" s="6">
+        <v>0</v>
+      </c>
+      <c r="F9" s="6">
+        <v>0</v>
+      </c>
+      <c r="G9" s="6">
+        <v>0</v>
+      </c>
+      <c r="H9" s="6">
+        <v>0</v>
+      </c>
+      <c r="I9" s="6">
+        <v>0</v>
+      </c>
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
@@ -934,11 +1039,21 @@
       <c r="D10" s="6">
         <v>0</v>
       </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
+      <c r="E10" s="6">
+        <v>0</v>
+      </c>
+      <c r="F10" s="6">
+        <v>0</v>
+      </c>
+      <c r="G10" s="6">
+        <v>0</v>
+      </c>
+      <c r="H10" s="6">
+        <v>0</v>
+      </c>
+      <c r="I10" s="6">
+        <v>0</v>
+      </c>
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
@@ -973,11 +1088,21 @@
         <f>(13/20)*10</f>
         <v>6.5</v>
       </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
+      <c r="E11" s="6">
+        <v>9.75</v>
+      </c>
+      <c r="F11" s="6">
+        <v>10</v>
+      </c>
+      <c r="G11" s="6">
+        <v>0</v>
+      </c>
+      <c r="H11" s="6">
+        <v>4</v>
+      </c>
+      <c r="I11" s="6">
+        <v>0</v>
+      </c>
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
@@ -1012,11 +1137,21 @@
         <f>(6/20)*10</f>
         <v>3</v>
       </c>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
+      <c r="E12" s="6">
+        <v>0</v>
+      </c>
+      <c r="F12" s="6">
+        <v>0</v>
+      </c>
+      <c r="G12" s="6">
+        <v>0</v>
+      </c>
+      <c r="H12" s="6">
+        <v>0</v>
+      </c>
+      <c r="I12" s="6">
+        <v>0</v>
+      </c>
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
@@ -1051,11 +1186,21 @@
         <f>(13/20)*10</f>
         <v>6.5</v>
       </c>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="4"/>
+      <c r="E13" s="6">
+        <v>10</v>
+      </c>
+      <c r="F13" s="6">
+        <v>10.5</v>
+      </c>
+      <c r="G13" s="6">
+        <v>10</v>
+      </c>
+      <c r="H13" s="6">
+        <v>0</v>
+      </c>
+      <c r="I13" s="4">
+        <v>0</v>
+      </c>
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
@@ -1089,11 +1234,21 @@
       <c r="D14" s="6">
         <v>0</v>
       </c>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
+      <c r="E14" s="6">
+        <v>0</v>
+      </c>
+      <c r="F14" s="6">
+        <v>0</v>
+      </c>
+      <c r="G14" s="6">
+        <v>0</v>
+      </c>
+      <c r="H14" s="6">
+        <v>0</v>
+      </c>
+      <c r="I14" s="6">
+        <v>0</v>
+      </c>
       <c r="J14" s="6"/>
       <c r="K14" s="6"/>
       <c r="L14" s="6"/>
@@ -1126,11 +1281,21 @@
       <c r="D15" s="18">
         <v>0</v>
       </c>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
+      <c r="E15" s="6">
+        <v>0</v>
+      </c>
+      <c r="F15" s="6">
+        <v>0</v>
+      </c>
+      <c r="G15" s="6">
+        <v>0</v>
+      </c>
+      <c r="H15" s="6">
+        <v>0</v>
+      </c>
+      <c r="I15" s="6">
+        <v>0</v>
+      </c>
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
       <c r="L15" s="6"/>
@@ -1183,7 +1348,7 @@
       </c>
       <c r="B17" s="8">
         <f>COUNTA(B1:Q1) * 10</f>
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -1241,7 +1406,7 @@
       </c>
       <c r="B22" s="13">
         <f>(SUM(B2:R2)/B17) * 40</f>
-        <v>14.666666666666666</v>
+        <v>29</v>
       </c>
       <c r="C22" s="14">
         <v>0</v>
@@ -1251,11 +1416,11 @@
       </c>
       <c r="E22" s="15">
         <f>B22+C22+D22</f>
-        <v>14.666666666666666</v>
+        <v>29</v>
       </c>
       <c r="F22" s="16">
         <f t="shared" ref="F22:F35" si="0">E22</f>
-        <v>14.666666666666666</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
@@ -1264,7 +1429,7 @@
       </c>
       <c r="B23" s="13">
         <f>(SUM(B3:R3)/B17) * 40</f>
-        <v>4.666666666666667</v>
+        <v>10.75</v>
       </c>
       <c r="C23" s="14">
         <v>0</v>
@@ -1274,11 +1439,11 @@
       </c>
       <c r="E23" s="15">
         <f t="shared" ref="E23:E35" si="1">B23+C23+D23</f>
-        <v>4.666666666666667</v>
+        <v>10.75</v>
       </c>
       <c r="F23" s="16">
         <f t="shared" si="0"/>
-        <v>4.666666666666667</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
@@ -1287,7 +1452,7 @@
       </c>
       <c r="B24" s="13">
         <f>(SUM(B4:R4)/B17) * 40</f>
-        <v>23.777777777777782</v>
+        <v>26.916666666666668</v>
       </c>
       <c r="C24" s="14">
         <v>0</v>
@@ -1297,11 +1462,11 @@
       </c>
       <c r="E24" s="15">
         <f t="shared" si="1"/>
-        <v>23.777777777777782</v>
+        <v>26.916666666666668</v>
       </c>
       <c r="F24" s="16">
         <f t="shared" si="0"/>
-        <v>23.777777777777782</v>
+        <v>26.916666666666668</v>
       </c>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.25">
@@ -1310,7 +1475,7 @@
       </c>
       <c r="B25" s="13">
         <f>(SUM(B5:R5)/B17) * 40</f>
-        <v>24.888888888888886</v>
+        <v>24.833333333333336</v>
       </c>
       <c r="C25" s="14">
         <v>0</v>
@@ -1320,11 +1485,11 @@
       </c>
       <c r="E25" s="15">
         <f t="shared" si="1"/>
-        <v>24.888888888888886</v>
+        <v>24.833333333333336</v>
       </c>
       <c r="F25" s="16">
         <f t="shared" si="0"/>
-        <v>24.888888888888886</v>
+        <v>24.833333333333336</v>
       </c>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
@@ -1333,7 +1498,7 @@
       </c>
       <c r="B26" s="13">
         <f>(SUM(B6:R6)/B17) * 40</f>
-        <v>24.222222222222221</v>
+        <v>35.083333333333329</v>
       </c>
       <c r="C26" s="14">
         <v>0</v>
@@ -1343,11 +1508,11 @@
       </c>
       <c r="E26" s="15">
         <f t="shared" si="1"/>
-        <v>24.222222222222221</v>
+        <v>35.083333333333329</v>
       </c>
       <c r="F26" s="16">
         <f t="shared" si="0"/>
-        <v>24.222222222222221</v>
+        <v>35.083333333333329</v>
       </c>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.25">
@@ -1356,7 +1521,7 @@
       </c>
       <c r="B27" s="13">
         <f>(SUM(B7:R7)/B17) * 40</f>
-        <v>28.444444444444446</v>
+        <v>36.166666666666671</v>
       </c>
       <c r="C27" s="14">
         <v>0</v>
@@ -1366,11 +1531,11 @@
       </c>
       <c r="E27" s="15">
         <f t="shared" si="1"/>
-        <v>28.444444444444446</v>
+        <v>36.166666666666671</v>
       </c>
       <c r="F27" s="16">
         <f t="shared" si="0"/>
-        <v>28.444444444444446</v>
+        <v>36.166666666666671</v>
       </c>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.25">
@@ -1402,7 +1567,7 @@
       </c>
       <c r="B29" s="13">
         <f>(SUM(B9:R9)/B17) * 40</f>
-        <v>6.6666666666666661</v>
+        <v>2.5</v>
       </c>
       <c r="C29" s="14">
         <v>0</v>
@@ -1412,11 +1577,11 @@
       </c>
       <c r="E29" s="15">
         <f t="shared" si="1"/>
-        <v>6.6666666666666661</v>
+        <v>2.5</v>
       </c>
       <c r="F29" s="16">
         <f t="shared" si="0"/>
-        <v>6.6666666666666661</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.25">
@@ -1425,7 +1590,7 @@
       </c>
       <c r="B30" s="13">
         <f>(SUM(B10:R10)/B17) * 40</f>
-        <v>17.111111111111114</v>
+        <v>6.416666666666667</v>
       </c>
       <c r="C30" s="14">
         <v>0</v>
@@ -1435,11 +1600,11 @@
       </c>
       <c r="E30" s="15">
         <f t="shared" si="1"/>
-        <v>17.111111111111114</v>
+        <v>6.416666666666667</v>
       </c>
       <c r="F30" s="16">
         <f t="shared" si="0"/>
-        <v>17.111111111111114</v>
+        <v>6.416666666666667</v>
       </c>
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.25">
@@ -1448,7 +1613,7 @@
       </c>
       <c r="B31" s="13">
         <f>(SUM(B11:R11)/B17) * 40</f>
-        <v>25.777777777777779</v>
+        <v>21.541666666666668</v>
       </c>
       <c r="C31" s="14">
         <v>0</v>
@@ -1458,11 +1623,11 @@
       </c>
       <c r="E31" s="15">
         <f t="shared" si="1"/>
-        <v>25.777777777777779</v>
+        <v>21.541666666666668</v>
       </c>
       <c r="F31" s="16">
         <f t="shared" si="0"/>
-        <v>25.777777777777779</v>
+        <v>21.541666666666668</v>
       </c>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.25">
@@ -1471,7 +1636,7 @@
       </c>
       <c r="B32" s="13">
         <f>(SUM(B12:R12)/B17) * 40</f>
-        <v>12.222222222222223</v>
+        <v>4.5833333333333339</v>
       </c>
       <c r="C32" s="14">
         <v>0</v>
@@ -1481,11 +1646,11 @@
       </c>
       <c r="E32" s="15">
         <f t="shared" si="1"/>
-        <v>12.222222222222223</v>
+        <v>4.5833333333333339</v>
       </c>
       <c r="F32" s="16">
         <f t="shared" si="0"/>
-        <v>12.222222222222223</v>
+        <v>4.5833333333333339</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1494,7 +1659,7 @@
       </c>
       <c r="B33" s="13">
         <f>(SUM(B13:R13)/B17) * 40</f>
-        <v>22.222222222222221</v>
+        <v>23.583333333333336</v>
       </c>
       <c r="C33" s="14">
         <v>0</v>
@@ -1504,11 +1669,11 @@
       </c>
       <c r="E33" s="15">
         <f t="shared" si="1"/>
-        <v>22.222222222222221</v>
+        <v>23.583333333333336</v>
       </c>
       <c r="F33" s="16">
         <f t="shared" si="0"/>
-        <v>22.222222222222221</v>
+        <v>23.583333333333336</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1517,7 +1682,7 @@
       </c>
       <c r="B34" s="13">
         <f>(SUM(B14:R14)/B17) * 40</f>
-        <v>10.888888888888889</v>
+        <v>4.0833333333333339</v>
       </c>
       <c r="C34" s="14">
         <v>0</v>
@@ -1527,11 +1692,11 @@
       </c>
       <c r="E34" s="15">
         <f t="shared" si="1"/>
-        <v>10.888888888888889</v>
+        <v>4.0833333333333339</v>
       </c>
       <c r="F34" s="16">
         <f t="shared" si="0"/>
-        <v>10.888888888888889</v>
+        <v>4.0833333333333339</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1540,7 +1705,7 @@
       </c>
       <c r="B35" s="13">
         <f>(SUM(B15:R15)/B17) * 40</f>
-        <v>10</v>
+        <v>3.75</v>
       </c>
       <c r="C35" s="14">
         <v>0</v>
@@ -1550,11 +1715,11 @@
       </c>
       <c r="E35" s="15">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>3.75</v>
       </c>
       <c r="F35" s="16">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>3.75</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
web 121 / quiz 05 & homework 11
</commit_message>
<xml_diff>
--- a/121/121.xlsx
+++ b/121/121.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24712"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alameheli\Desktop\scores\121\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MFT\004-scores\121\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F4CE847-EDAA-43F2-94AF-9EE282C68101}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9BF053D-57C4-4725-8058-23CDC30A87D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="web 121" sheetId="1" r:id="rId1"/>
@@ -20,11 +20,8 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -35,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>No.</t>
   </si>
@@ -83,6 +80,9 @@
   </si>
   <si>
     <t>Q04</t>
+  </si>
+  <si>
+    <t>Q05</t>
   </si>
 </sst>
 </file>
@@ -589,8 +589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -640,7 +640,9 @@
       <c r="J1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="2"/>
+      <c r="K1" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
@@ -679,10 +681,13 @@
         <v>10</v>
       </c>
       <c r="J2" s="4">
-        <f>(10/18)*10</f>
-        <v>5.5555555555555554</v>
-      </c>
-      <c r="K2" s="4"/>
+        <f>(10/17)*10</f>
+        <v>5.882352941176471</v>
+      </c>
+      <c r="K2" s="4">
+        <f>(24/35)*10</f>
+        <v>6.8571428571428577</v>
+      </c>
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
@@ -729,10 +734,13 @@
         <v>0</v>
       </c>
       <c r="J3" s="4">
-        <f>(9/18)*10</f>
-        <v>5</v>
-      </c>
-      <c r="K3" s="4"/>
+        <f>(9/17)*10</f>
+        <v>5.2941176470588234</v>
+      </c>
+      <c r="K3" s="4">
+        <f>(23/35)*10</f>
+        <v>6.5714285714285712</v>
+      </c>
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
       <c r="N3" s="4"/>
@@ -778,13 +786,16 @@
         <v>9.5</v>
       </c>
       <c r="I4" s="4">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J4" s="4">
-        <f>(11/18)*10</f>
-        <v>6.1111111111111116</v>
-      </c>
-      <c r="K4" s="4"/>
+        <f>(11/17)*10</f>
+        <v>6.4705882352941178</v>
+      </c>
+      <c r="K4" s="4">
+        <f>(29/35)*10</f>
+        <v>8.2857142857142865</v>
+      </c>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
       <c r="N4" s="6"/>
@@ -827,16 +838,19 @@
         <v>10</v>
       </c>
       <c r="H5" s="4">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I5" s="4">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J5" s="4">
-        <f>(10/18)*10</f>
-        <v>5.5555555555555554</v>
-      </c>
-      <c r="K5" s="4"/>
+        <f>(10/17)*10</f>
+        <v>5.882352941176471</v>
+      </c>
+      <c r="K5" s="4">
+        <f>(23/35)*10</f>
+        <v>6.5714285714285712</v>
+      </c>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
       <c r="N5" s="6"/>
@@ -885,10 +899,13 @@
         <v>10</v>
       </c>
       <c r="J6" s="4">
-        <f>(11/18)*10</f>
-        <v>6.1111111111111116</v>
-      </c>
-      <c r="K6" s="4"/>
+        <f>(11/17)*10</f>
+        <v>6.4705882352941178</v>
+      </c>
+      <c r="K6" s="4">
+        <f>(32/35)*10</f>
+        <v>9.1428571428571423</v>
+      </c>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
       <c r="N6" s="6"/>
@@ -937,10 +954,12 @@
         <v>10</v>
       </c>
       <c r="J7" s="6">
-        <f>(13/18)*10</f>
-        <v>7.2222222222222223</v>
-      </c>
-      <c r="K7" s="6"/>
+        <f>(13/17)*10</f>
+        <v>7.6470588235294112</v>
+      </c>
+      <c r="K7" s="6">
+        <v>0</v>
+      </c>
       <c r="L7" s="6"/>
       <c r="M7" s="6"/>
       <c r="N7" s="6"/>
@@ -988,7 +1007,9 @@
       <c r="J8" s="6">
         <v>0</v>
       </c>
-      <c r="K8" s="6"/>
+      <c r="K8" s="6">
+        <v>0</v>
+      </c>
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
       <c r="N8" s="6"/>
@@ -1037,7 +1058,9 @@
       <c r="J9" s="6">
         <v>0</v>
       </c>
-      <c r="K9" s="6"/>
+      <c r="K9" s="6">
+        <v>0</v>
+      </c>
       <c r="L9" s="6"/>
       <c r="M9" s="6"/>
       <c r="N9" s="6"/>
@@ -1087,7 +1110,9 @@
       <c r="J10" s="6">
         <v>0</v>
       </c>
-      <c r="K10" s="6"/>
+      <c r="K10" s="6">
+        <v>0</v>
+      </c>
       <c r="L10" s="6"/>
       <c r="M10" s="6"/>
       <c r="N10" s="6"/>
@@ -1136,10 +1161,12 @@
         <v>0</v>
       </c>
       <c r="J11" s="6">
-        <f>(11/18)*10</f>
-        <v>6.1111111111111116</v>
-      </c>
-      <c r="K11" s="6"/>
+        <f>(11/17)*10</f>
+        <v>6.4705882352941178</v>
+      </c>
+      <c r="K11" s="6">
+        <v>0</v>
+      </c>
       <c r="L11" s="6"/>
       <c r="M11" s="6"/>
       <c r="N11" s="6"/>
@@ -1190,7 +1217,9 @@
       <c r="J12" s="6">
         <v>0</v>
       </c>
-      <c r="K12" s="6"/>
+      <c r="K12" s="6">
+        <v>0</v>
+      </c>
       <c r="L12" s="6"/>
       <c r="M12" s="6"/>
       <c r="N12" s="6"/>
@@ -1233,16 +1262,18 @@
         <v>10</v>
       </c>
       <c r="H13" s="6">
-        <v>0</v>
+        <v>8.5</v>
       </c>
       <c r="I13" s="4">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J13" s="6">
-        <f>(11/18)*10</f>
-        <v>6.1111111111111116</v>
-      </c>
-      <c r="K13" s="6"/>
+        <f>(11/17)*10</f>
+        <v>6.4705882352941178</v>
+      </c>
+      <c r="K13" s="6">
+        <v>0</v>
+      </c>
       <c r="L13" s="6"/>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
@@ -1290,10 +1321,13 @@
         <v>0</v>
       </c>
       <c r="J14" s="6">
-        <f>(5/18)*10</f>
-        <v>2.7777777777777777</v>
-      </c>
-      <c r="K14" s="6"/>
+        <f>(5/17)*10</f>
+        <v>2.9411764705882355</v>
+      </c>
+      <c r="K14" s="6">
+        <f>(14/35)*10</f>
+        <v>4</v>
+      </c>
       <c r="L14" s="6"/>
       <c r="M14" s="6"/>
       <c r="N14" s="6"/>
@@ -1342,7 +1376,9 @@
       <c r="J15" s="6">
         <v>0</v>
       </c>
-      <c r="K15" s="6"/>
+      <c r="K15" s="6">
+        <v>0</v>
+      </c>
       <c r="L15" s="6"/>
       <c r="M15" s="6"/>
       <c r="N15" s="6"/>
@@ -1393,7 +1429,7 @@
       </c>
       <c r="B17" s="8">
         <f>COUNTA(B1:Q1) * 10</f>
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -1451,21 +1487,21 @@
       </c>
       <c r="B22" s="13">
         <f>(SUM(B2:R2)/B17) * 40</f>
-        <v>28.246913580246911</v>
+        <v>28.29579831932773</v>
       </c>
       <c r="C22" s="14">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D22" s="14">
         <v>0</v>
       </c>
       <c r="E22" s="15">
         <f>B22+C22+D22</f>
-        <v>28.246913580246911</v>
+        <v>36.29579831932773</v>
       </c>
       <c r="F22" s="16">
         <f t="shared" ref="F22:F35" si="0">E22</f>
-        <v>28.246913580246911</v>
+        <v>36.29579831932773</v>
       </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
@@ -1474,21 +1510,21 @@
       </c>
       <c r="B23" s="13">
         <f>(SUM(B3:R3)/B17) * 40</f>
-        <v>11.777777777777779</v>
+        <v>13.346218487394959</v>
       </c>
       <c r="C23" s="14">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D23" s="14">
         <v>0</v>
       </c>
       <c r="E23" s="15">
         <f t="shared" ref="E23:E35" si="1">B23+C23+D23</f>
-        <v>11.777777777777779</v>
+        <v>20.346218487394957</v>
       </c>
       <c r="F23" s="16">
         <f t="shared" si="0"/>
-        <v>11.777777777777779</v>
+        <v>20.346218487394957</v>
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
@@ -1497,21 +1533,21 @@
       </c>
       <c r="B24" s="13">
         <f>(SUM(B4:R4)/B17) * 40</f>
-        <v>26.641975308641975</v>
+        <v>31.4358543417367</v>
       </c>
       <c r="C24" s="14">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D24" s="14">
         <v>0</v>
       </c>
       <c r="E24" s="15">
         <f t="shared" si="1"/>
-        <v>26.641975308641975</v>
+        <v>40.4358543417367</v>
       </c>
       <c r="F24" s="16">
         <f t="shared" si="0"/>
-        <v>26.641975308641975</v>
+        <v>40.4358543417367</v>
       </c>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.25">
@@ -1520,21 +1556,21 @@
       </c>
       <c r="B25" s="13">
         <f>(SUM(B5:R5)/B17) * 40</f>
-        <v>24.543209876543209</v>
+        <v>32.848179271708673</v>
       </c>
       <c r="C25" s="14">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D25" s="14">
         <v>0</v>
       </c>
       <c r="E25" s="15">
         <f t="shared" si="1"/>
-        <v>24.543209876543209</v>
+        <v>40.848179271708673</v>
       </c>
       <c r="F25" s="16">
         <f t="shared" si="0"/>
-        <v>24.543209876543209</v>
+        <v>40.848179271708673</v>
       </c>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
@@ -1543,21 +1579,21 @@
       </c>
       <c r="B26" s="13">
         <f>(SUM(B6:R6)/B17) * 40</f>
-        <v>33.901234567901227</v>
+        <v>34.312044817927166</v>
       </c>
       <c r="C26" s="14">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D26" s="14">
         <v>0</v>
       </c>
       <c r="E26" s="15">
         <f t="shared" si="1"/>
-        <v>33.901234567901227</v>
+        <v>44.312044817927166</v>
       </c>
       <c r="F26" s="16">
         <f t="shared" si="0"/>
-        <v>33.901234567901227</v>
+        <v>44.312044817927166</v>
       </c>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.25">
@@ -1566,21 +1602,21 @@
       </c>
       <c r="B27" s="13">
         <f>(SUM(B7:R7)/B17) * 40</f>
-        <v>35.358024691358032</v>
+        <v>31.992156862745098</v>
       </c>
       <c r="C27" s="14">
-        <v>0</v>
+        <v>9.5</v>
       </c>
       <c r="D27" s="14">
         <v>0</v>
       </c>
       <c r="E27" s="15">
         <f t="shared" si="1"/>
-        <v>35.358024691358032</v>
+        <v>41.492156862745098</v>
       </c>
       <c r="F27" s="16">
         <f t="shared" si="0"/>
-        <v>35.358024691358032</v>
+        <v>41.492156862745098</v>
       </c>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.25">
@@ -1612,21 +1648,21 @@
       </c>
       <c r="B29" s="13">
         <f>(SUM(B9:R9)/B17) * 40</f>
-        <v>2.2222222222222223</v>
+        <v>2</v>
       </c>
       <c r="C29" s="14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D29" s="14">
         <v>0</v>
       </c>
       <c r="E29" s="15">
         <f t="shared" si="1"/>
-        <v>2.2222222222222223</v>
+        <v>5</v>
       </c>
       <c r="F29" s="16">
         <f t="shared" si="0"/>
-        <v>2.2222222222222223</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.25">
@@ -1635,21 +1671,21 @@
       </c>
       <c r="B30" s="13">
         <f>(SUM(B10:R10)/B17) * 40</f>
-        <v>5.7037037037037042</v>
+        <v>5.1333333333333329</v>
       </c>
       <c r="C30" s="14">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D30" s="14">
         <v>0</v>
       </c>
       <c r="E30" s="15">
         <f t="shared" si="1"/>
-        <v>5.7037037037037042</v>
+        <v>9.1333333333333329</v>
       </c>
       <c r="F30" s="16">
         <f t="shared" si="0"/>
-        <v>5.7037037037037042</v>
+        <v>9.1333333333333329</v>
       </c>
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.25">
@@ -1658,21 +1694,21 @@
       </c>
       <c r="B31" s="13">
         <f>(SUM(B11:R11)/B17) * 40</f>
-        <v>21.864197530864196</v>
+        <v>19.821568627450979</v>
       </c>
       <c r="C31" s="14">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D31" s="14">
         <v>0</v>
       </c>
       <c r="E31" s="15">
         <f t="shared" si="1"/>
-        <v>21.864197530864196</v>
+        <v>26.821568627450979</v>
       </c>
       <c r="F31" s="16">
         <f t="shared" si="0"/>
-        <v>21.864197530864196</v>
+        <v>26.821568627450979</v>
       </c>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.25">
@@ -1681,21 +1717,21 @@
       </c>
       <c r="B32" s="13">
         <f>(SUM(B12:R12)/B17) * 40</f>
-        <v>4.0740740740740744</v>
+        <v>3.666666666666667</v>
       </c>
       <c r="C32" s="14">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D32" s="14">
         <v>0</v>
       </c>
       <c r="E32" s="15">
         <f t="shared" si="1"/>
-        <v>4.0740740740740744</v>
+        <v>11.666666666666668</v>
       </c>
       <c r="F32" s="16">
         <f t="shared" si="0"/>
-        <v>4.0740740740740744</v>
+        <v>11.666666666666668</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1704,21 +1740,21 @@
       </c>
       <c r="B33" s="13">
         <f>(SUM(B13:R13)/B17) * 40</f>
-        <v>23.67901234567902</v>
+        <v>28.854901960784318</v>
       </c>
       <c r="C33" s="14">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D33" s="14">
         <v>0</v>
       </c>
       <c r="E33" s="15">
         <f t="shared" si="1"/>
-        <v>23.67901234567902</v>
+        <v>37.854901960784318</v>
       </c>
       <c r="F33" s="16">
         <f t="shared" si="0"/>
-        <v>23.67901234567902</v>
+        <v>37.854901960784318</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1727,21 +1763,21 @@
       </c>
       <c r="B34" s="13">
         <f>(SUM(B14:R14)/B17) * 40</f>
-        <v>17.530864197530867</v>
+        <v>17.443137254901963</v>
       </c>
       <c r="C34" s="14">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D34" s="14">
         <v>0</v>
       </c>
       <c r="E34" s="15">
         <f t="shared" si="1"/>
-        <v>17.530864197530867</v>
+        <v>23.443137254901963</v>
       </c>
       <c r="F34" s="16">
         <f t="shared" si="0"/>
-        <v>17.530864197530867</v>
+        <v>23.443137254901963</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1750,21 +1786,21 @@
       </c>
       <c r="B35" s="13">
         <f>(SUM(B15:R15)/B17) * 40</f>
-        <v>3.333333333333333</v>
+        <v>3</v>
       </c>
       <c r="C35" s="14">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D35" s="14">
         <v>0</v>
       </c>
       <c r="E35" s="15">
         <f t="shared" si="1"/>
-        <v>3.333333333333333</v>
+        <v>10</v>
       </c>
       <c r="F35" s="16">
         <f t="shared" si="0"/>
-        <v>3.333333333333333</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
web-121 / final scores
</commit_message>
<xml_diff>
--- a/121/121.xlsx
+++ b/121/121.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MFT\004-scores\121\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9BF053D-57C4-4725-8058-23CDC30A87D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C7DE1E-77B1-47B2-A5CB-DC503D41FD0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3135" yWindow="2640" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="web 121" sheetId="1" r:id="rId1"/>
@@ -590,7 +590,7 @@
   <dimension ref="A1:Z37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -725,13 +725,13 @@
         <v>9.5</v>
       </c>
       <c r="G3" s="4">
-        <v>0</v>
+        <v>9.5</v>
       </c>
       <c r="H3" s="4">
         <v>0</v>
       </c>
       <c r="I3" s="4">
-        <v>0</v>
+        <v>9.5</v>
       </c>
       <c r="J3" s="4">
         <f>(9/17)*10</f>
@@ -1291,43 +1291,17 @@
       <c r="Z13" s="5"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
-        <v>13</v>
-      </c>
-      <c r="B14" s="6">
-        <f>(4/10)*10</f>
-        <v>4</v>
-      </c>
-      <c r="C14" s="6">
-        <f>(5/12)*10</f>
-        <v>4.166666666666667</v>
-      </c>
-      <c r="D14" s="6">
-        <v>0</v>
-      </c>
-      <c r="E14" s="6">
-        <v>10</v>
-      </c>
-      <c r="F14" s="6">
-        <v>10</v>
-      </c>
-      <c r="G14" s="6">
-        <v>8.5</v>
-      </c>
-      <c r="H14" s="6">
-        <v>0</v>
-      </c>
-      <c r="I14" s="6">
-        <v>0</v>
-      </c>
-      <c r="J14" s="6">
-        <f>(5/17)*10</f>
-        <v>2.9411764705882355</v>
-      </c>
-      <c r="K14" s="6">
-        <f>(14/35)*10</f>
-        <v>4</v>
-      </c>
+      <c r="A14" s="3"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
       <c r="L14" s="6"/>
       <c r="M14" s="6"/>
       <c r="N14" s="6"/>
@@ -1493,15 +1467,15 @@
         <v>8</v>
       </c>
       <c r="D22" s="14">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="E22" s="15">
         <f>B22+C22+D22</f>
-        <v>36.29579831932773</v>
+        <v>81.29579831932773</v>
       </c>
       <c r="F22" s="16">
         <f t="shared" ref="F22:F35" si="0">E22</f>
-        <v>36.29579831932773</v>
+        <v>81.29579831932773</v>
       </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
@@ -1510,7 +1484,7 @@
       </c>
       <c r="B23" s="13">
         <f>(SUM(B3:R3)/B17) * 40</f>
-        <v>13.346218487394959</v>
+        <v>20.946218487394958</v>
       </c>
       <c r="C23" s="14">
         <v>7</v>
@@ -1520,11 +1494,11 @@
       </c>
       <c r="E23" s="15">
         <f t="shared" ref="E23:E35" si="1">B23+C23+D23</f>
-        <v>20.346218487394957</v>
+        <v>27.946218487394958</v>
       </c>
       <c r="F23" s="16">
         <f t="shared" si="0"/>
-        <v>20.346218487394957</v>
+        <v>27.946218487394958</v>
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
@@ -1562,15 +1536,15 @@
         <v>8</v>
       </c>
       <c r="D25" s="14">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="E25" s="15">
         <f t="shared" si="1"/>
-        <v>40.848179271708673</v>
+        <v>90.848179271708673</v>
       </c>
       <c r="F25" s="16">
         <f t="shared" si="0"/>
-        <v>40.848179271708673</v>
+        <v>90.848179271708673</v>
       </c>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
@@ -1585,15 +1559,15 @@
         <v>10</v>
       </c>
       <c r="D26" s="14">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="E26" s="15">
         <f t="shared" si="1"/>
-        <v>44.312044817927166</v>
+        <v>100.31204481792716</v>
       </c>
       <c r="F26" s="16">
         <f t="shared" si="0"/>
-        <v>44.312044817927166</v>
+        <v>100.31204481792716</v>
       </c>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.25">
@@ -1608,15 +1582,15 @@
         <v>9.5</v>
       </c>
       <c r="D27" s="14">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="E27" s="15">
         <f t="shared" si="1"/>
-        <v>41.492156862745098</v>
+        <v>91.492156862745105</v>
       </c>
       <c r="F27" s="16">
         <f t="shared" si="0"/>
-        <v>41.492156862745098</v>
+        <v>91.492156862745105</v>
       </c>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.25">
@@ -1746,39 +1720,24 @@
         <v>9</v>
       </c>
       <c r="D33" s="14">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="E33" s="15">
         <f t="shared" si="1"/>
-        <v>37.854901960784318</v>
+        <v>91.854901960784318</v>
       </c>
       <c r="F33" s="16">
         <f t="shared" si="0"/>
-        <v>37.854901960784318</v>
+        <v>91.854901960784318</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="10">
-        <v>13</v>
-      </c>
-      <c r="B34" s="13">
-        <f>(SUM(B14:R14)/B17) * 40</f>
-        <v>17.443137254901963</v>
-      </c>
-      <c r="C34" s="14">
-        <v>6</v>
-      </c>
-      <c r="D34" s="14">
-        <v>0</v>
-      </c>
-      <c r="E34" s="15">
-        <f t="shared" si="1"/>
-        <v>23.443137254901963</v>
-      </c>
-      <c r="F34" s="16">
-        <f t="shared" si="0"/>
-        <v>23.443137254901963</v>
-      </c>
+      <c r="A34" s="10"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="16"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="10">

</xml_diff>

<commit_message>
web 121 / updated
</commit_message>
<xml_diff>
--- a/121/121.xlsx
+++ b/121/121.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MFT\004-scores\121\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alameheli\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C7DE1E-77B1-47B2-A5CB-DC503D41FD0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CEDE5BD-0305-4E4D-A4D6-919D00D774E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3135" yWindow="2640" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="web 121" sheetId="1" r:id="rId1"/>
@@ -20,8 +20,11 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -590,7 +593,7 @@
   <dimension ref="A1:Z37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1291,17 +1294,43 @@
       <c r="Z13" s="5"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
+      <c r="A14" s="3">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6">
+        <f>(4/10)*10</f>
+        <v>4</v>
+      </c>
+      <c r="C14" s="6">
+        <f>(5/12)*10</f>
+        <v>4.166666666666667</v>
+      </c>
+      <c r="D14" s="6">
+        <v>0</v>
+      </c>
+      <c r="E14" s="6">
+        <v>10</v>
+      </c>
+      <c r="F14" s="6">
+        <v>10</v>
+      </c>
+      <c r="G14" s="6">
+        <v>8.5</v>
+      </c>
+      <c r="H14" s="6">
+        <v>5</v>
+      </c>
+      <c r="I14" s="6">
+        <v>5</v>
+      </c>
+      <c r="J14" s="6">
+        <f>(5/17)*10</f>
+        <v>2.9411764705882355</v>
+      </c>
+      <c r="K14" s="6">
+        <f>(14/35)*10</f>
+        <v>4</v>
+      </c>
       <c r="L14" s="6"/>
       <c r="M14" s="6"/>
       <c r="N14" s="6"/>
@@ -1732,12 +1761,27 @@
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="10"/>
-      <c r="B34" s="13"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="15"/>
-      <c r="F34" s="16"/>
+      <c r="A34" s="10">
+        <v>13</v>
+      </c>
+      <c r="B34" s="13">
+        <f>(SUM(B14:R14)/B17) * 40</f>
+        <v>21.443137254901963</v>
+      </c>
+      <c r="C34" s="14">
+        <v>5</v>
+      </c>
+      <c r="D34" s="14">
+        <v>0</v>
+      </c>
+      <c r="E34" s="15">
+        <f t="shared" si="1"/>
+        <v>26.443137254901963</v>
+      </c>
+      <c r="F34" s="16">
+        <f t="shared" si="0"/>
+        <v>26.443137254901963</v>
+      </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="10">

</xml_diff>